<commit_message>
added row number to error log
</commit_message>
<xml_diff>
--- a/Application/ErrorData.xlsx
+++ b/Application/ErrorData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>year</t>
   </si>
@@ -26,6 +26,9 @@
     <t>coverage_type</t>
   </si>
   <si>
+    <t>row_number</t>
+  </si>
+  <si>
     <t>error_message</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
     <t>Part D</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>brand_name cannot be empty or null.</t>
   </si>
   <si>
@@ -50,6 +56,9 @@
     <t>Part E</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>2012</t>
   </si>
   <si>
@@ -59,16 +68,28 @@
     <t>Part B</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>2011</t>
   </si>
   <si>
     <t>Albuterol Sulfate</t>
   </si>
   <si>
+    <t>14</t>
+  </si>
+  <si>
     <t>2014</t>
   </si>
   <si>
+    <t>17</t>
+  </si>
+  <si>
     <t>Fluticasone/Salmeterol</t>
+  </si>
+  <si>
+    <t>25</t>
   </si>
 </sst>
 </file>
@@ -113,7 +134,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -135,107 +156,128 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>